<commit_message>
ajout du plan de test, et divisions des principales fonctions en plusieurs sous-fonctions, factoring
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drakmirr\Desktop\P5OC\JWDP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25241A3-AD81-47A1-9B60-4993FC436D51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3D4192-A7B7-472C-AA51-E53C418EDFEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3855" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="118">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -49,9 +49,6 @@
     <t>cams</t>
   </si>
   <si>
-    <t>panier.js</t>
-  </si>
-  <si>
     <t>ajouterAuPanier</t>
   </si>
   <si>
@@ -76,30 +73,9 @@
     <t>tableauRecapPanier</t>
   </si>
   <si>
-    <t>connectionApi.js</t>
-  </si>
-  <si>
-    <t>liste.js</t>
-  </si>
-  <si>
-    <t>1 à 41</t>
-  </si>
-  <si>
-    <t>produits.js</t>
-  </si>
-  <si>
     <t>detailsCam</t>
   </si>
   <si>
-    <t>formulaire.js</t>
-  </si>
-  <si>
-    <t>23 à 89</t>
-  </si>
-  <si>
-    <t>1 à 74</t>
-  </si>
-  <si>
     <t>supprimerDuPanier</t>
   </si>
   <si>
@@ -112,9 +88,6 @@
     <t>8 à 16</t>
   </si>
   <si>
-    <t>44 à 149</t>
-  </si>
-  <si>
     <t>envoiApi.js</t>
   </si>
   <si>
@@ -125,13 +98,289 @@
   </si>
   <si>
     <t>recupOrderId</t>
+  </si>
+  <si>
+    <t>connexionApi.js</t>
+  </si>
+  <si>
+    <t>la fonction doit se connecter à l'api</t>
+  </si>
+  <si>
+    <t>la fonction doit afficher un compteur qui comptabilise les éléments du panier</t>
+  </si>
+  <si>
+    <t>la fonction doit ajouter le produit sélectionné dans le panierClient</t>
+  </si>
+  <si>
+    <t>la fonction doit supprimer le produit sélectionné du panierClient</t>
+  </si>
+  <si>
+    <t>La fonction doit créer un objet de stockage pour le panier s'il n'existe pas</t>
+  </si>
+  <si>
+    <t>La fonction envoi une requete API POST et doit retourner un objet contact avec l'orderId</t>
+  </si>
+  <si>
+    <t>retourner dans un console.log l'etat de la requete à l'aide la propriété readystate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reponse retourné differente 4 correspondant à une mauvaise connexion ou autre selon le status </t>
+  </si>
+  <si>
+    <t>liste2.js</t>
+  </si>
+  <si>
+    <t>creationElementListe</t>
+  </si>
+  <si>
+    <t>les elements doivent s'afficher sur la page html</t>
+  </si>
+  <si>
+    <t>22 à 29</t>
+  </si>
+  <si>
+    <t>32 à 42</t>
+  </si>
+  <si>
+    <t>ajoutAttributsCardListe</t>
+  </si>
+  <si>
+    <t>la fonction doit créer les balises html nécessaire à chaque card</t>
+  </si>
+  <si>
+    <t>la fonction ajoute les differents attributs sur les balises crées</t>
+  </si>
+  <si>
+    <t>les attributs doivents apparaitre sur les balises en html</t>
+  </si>
+  <si>
+    <t>les balises ne sont pas créer</t>
+  </si>
+  <si>
+    <t>les attributs ne sont pas ajoutés</t>
+  </si>
+  <si>
+    <t>46 à 50</t>
+  </si>
+  <si>
+    <t>positionHtml</t>
+  </si>
+  <si>
+    <t>la fonction agence la structure html des balises crées</t>
+  </si>
+  <si>
+    <t>verifier la structure html et verifier l'affichage des cards sur la page web</t>
+  </si>
+  <si>
+    <t>agencement/positionnement des balises html non réalisé</t>
+  </si>
+  <si>
+    <t>ajoutContenuCardListe</t>
+  </si>
+  <si>
+    <t>53 à 57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction ajoute le contenu textuel des cards </t>
+  </si>
+  <si>
+    <t>verifier sur la page web l'affichage du contenu</t>
+  </si>
+  <si>
+    <t>le contenu n'est pas ajouté</t>
+  </si>
+  <si>
+    <t>13 à 59</t>
+  </si>
+  <si>
+    <t>la fonction appel les 4 fonctions necessaires à la creation des cards</t>
+  </si>
+  <si>
+    <t>verifier l'affichage des cards sur la page web</t>
+  </si>
+  <si>
+    <t>mauvais affichage ou affichage absent des cards</t>
+  </si>
+  <si>
+    <t>panier3.js</t>
+  </si>
+  <si>
+    <t>verifier l'existence l'objet dans le localstorage</t>
+  </si>
+  <si>
+    <t>l'objet n'est pas créer</t>
+  </si>
+  <si>
+    <t>verifier sur la page web l'affichage du compteur</t>
+  </si>
+  <si>
+    <t>le compteur n'apparait pas ou ne comptabilise pas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verifier sur la pge web si le produit a été ajouté et/ou le panierClient dans le localstorage </t>
+  </si>
+  <si>
+    <t>le produit n'est pas ajouté</t>
+  </si>
+  <si>
+    <t>verifier sur la page web la suppression effective</t>
+  </si>
+  <si>
+    <t>le produit n'est pas supprimé</t>
+  </si>
+  <si>
+    <t>creationElementPanier</t>
+  </si>
+  <si>
+    <t>la fonction doit créer les balises html nécessaire au tableau panier</t>
+  </si>
+  <si>
+    <t>positionHtmlPanier</t>
+  </si>
+  <si>
+    <t>verifier la structure html et verifier l'affichage du tableau panier sur la page web</t>
+  </si>
+  <si>
+    <t>64 à 71</t>
+  </si>
+  <si>
+    <t>ajoutAttributs</t>
+  </si>
+  <si>
+    <t>76 à 80</t>
+  </si>
+  <si>
+    <t>84 à 88</t>
+  </si>
+  <si>
+    <t>ajoutContenuCellule</t>
+  </si>
+  <si>
+    <t>la fonction ajoute le contenu textuel du tableau panier</t>
+  </si>
+  <si>
+    <t>92 à 98</t>
+  </si>
+  <si>
+    <t>ajoutContenuPanier</t>
+  </si>
+  <si>
+    <t>104 à 107</t>
+  </si>
+  <si>
+    <t>la fonction ajoute le contenu du panier dans l'objet produit</t>
+  </si>
+  <si>
+    <t>verifier le contenu de l'objeet produit</t>
+  </si>
+  <si>
+    <t>la fonction fait appel aux 5 fonctions necessaires à la creation du tableau</t>
+  </si>
+  <si>
+    <t>verifier sur la page web l'affichage et le contenu du tableau</t>
+  </si>
+  <si>
+    <t>mauvais affichage ou affichage absent du tableau</t>
+  </si>
+  <si>
+    <t>produitCard.js</t>
+  </si>
+  <si>
+    <t>attributCardProduit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction ajoute les differents attributs sur les balises </t>
+  </si>
+  <si>
+    <t>17 à 21</t>
+  </si>
+  <si>
+    <t>26 à 32</t>
+  </si>
+  <si>
+    <t>ajoutContenuProduitCard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction ajoute le contenu textuel de la card </t>
+  </si>
+  <si>
+    <t>12 à 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fonction appel 3 fonctions necessaires à l'affichage de la card </t>
+  </si>
+  <si>
+    <t>verifier l'affichage de la card sur la page web</t>
+  </si>
+  <si>
+    <t>affichage défaillant ou absent sur la page web</t>
+  </si>
+  <si>
+    <t>formulaire2.js</t>
+  </si>
+  <si>
+    <t>verifInput</t>
+  </si>
+  <si>
+    <t>21 à 30</t>
+  </si>
+  <si>
+    <t>La fonction doit vérifier le bon formatage des données de l'input ert affiche la couleur correspondante vert ou rouge</t>
+  </si>
+  <si>
+    <t>on saisi des mots dans l'input pour verifier la couleur affichée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la couleur affiché ne correspond pas </t>
+  </si>
+  <si>
+    <t>33 à 46</t>
+  </si>
+  <si>
+    <t>enableButtonValidation</t>
+  </si>
+  <si>
+    <t>La fontion doit activer le bouton validation si tous les input passe au vert</t>
+  </si>
+  <si>
+    <t>on valide tous les inputs</t>
+  </si>
+  <si>
+    <t>le bouton ne s'active pas</t>
+  </si>
+  <si>
+    <t>48 à 55</t>
+  </si>
+  <si>
+    <t>la fonction appel la fonction verifInput sur chaque input et la fonction enableButtonValidation</t>
+  </si>
+  <si>
+    <t>verifier les inputs et le bouton validation sur le formulaire</t>
+  </si>
+  <si>
+    <t>la fonvtion verifInput n'est pas appliqué sur chaque input</t>
+  </si>
+  <si>
+    <t>la requete n'abouti pas</t>
+  </si>
+  <si>
+    <t>envoyer le formulaire et verifier la reponse</t>
+  </si>
+  <si>
+    <t>verifier l'apparition de l'orderId sur la page web</t>
+  </si>
+  <si>
+    <t>La fonction doit récuperer l'orderID du sessionStorage et l'afficher sur la page web</t>
+  </si>
+  <si>
+    <t>l'orderId n'est pas recupérer et/ou n'est pas afficher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -151,8 +400,19 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,8 +425,50 @@
         <bgColor rgb="FFD9D2E9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -174,11 +476,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -195,6 +512,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,25 +745,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="50.5703125" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" customWidth="1"/>
     <col min="6" max="6" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -476,8 +808,8 @@
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>18</v>
+      <c r="A3" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -485,241 +817,499 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="4:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="4:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="4:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -784,67 +1374,67 @@
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
-    <row r="55" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
-    <row r="56" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -5554,7 +6144,73 @@
       <c r="E998" s="4"/>
       <c r="F998" s="4"/>
     </row>
+    <row r="999" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D999" s="4"/>
+      <c r="E999" s="4"/>
+      <c r="F999" s="4"/>
+    </row>
+    <row r="1000" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1000" s="4"/>
+      <c r="E1000" s="4"/>
+      <c r="F1000" s="4"/>
+    </row>
+    <row r="1001" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1001" s="4"/>
+      <c r="E1001" s="4"/>
+      <c r="F1001" s="4"/>
+    </row>
+    <row r="1002" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1002" s="4"/>
+      <c r="E1002" s="4"/>
+      <c r="F1002" s="4"/>
+    </row>
+    <row r="1003" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1003" s="4"/>
+      <c r="E1003" s="4"/>
+      <c r="F1003" s="4"/>
+    </row>
+    <row r="1004" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1004" s="4"/>
+      <c r="E1004" s="4"/>
+      <c r="F1004" s="4"/>
+    </row>
+    <row r="1005" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1005" s="4"/>
+      <c r="E1005" s="4"/>
+      <c r="F1005" s="4"/>
+    </row>
+    <row r="1006" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1006" s="4"/>
+      <c r="E1006" s="4"/>
+      <c r="F1006" s="4"/>
+    </row>
+    <row r="1007" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1007" s="4"/>
+      <c r="E1007" s="4"/>
+      <c r="F1007" s="4"/>
+    </row>
+    <row r="1008" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1008" s="4"/>
+      <c r="E1008" s="4"/>
+      <c r="F1008" s="4"/>
+    </row>
+    <row r="1009" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1009" s="4"/>
+      <c r="E1009" s="4"/>
+      <c r="F1009" s="4"/>
+    </row>
+    <row r="1010" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1010" s="4"/>
+      <c r="E1010" s="4"/>
+      <c r="F1010" s="4"/>
+    </row>
+    <row r="1011" spans="4:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D1011" s="4"/>
+      <c r="E1011" s="4"/>
+      <c r="F1011" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
optimisation du produitCard.js grace aux promise et connection à l'api via fetch
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drakmirr\Desktop\P5OC\JWDP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3D4192-A7B7-472C-AA51-E53C418EDFEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D4B885-D1EF-4FC4-8FE2-43C24A3C70B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3855" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="120">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t>l'orderId n'est pas recupérer et/ou n'est pas afficher</t>
+  </si>
+  <si>
+    <t>a modifier précision</t>
+  </si>
+  <si>
+    <t>nommer les 4 fonctions</t>
   </si>
 </sst>
 </file>
@@ -495,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,6 +533,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,8 +757,8 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -826,6 +835,9 @@
       <c r="F3" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="G3" s="17" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -925,6 +937,9 @@
       </c>
       <c r="F8" s="5" t="s">
         <v>59</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modification des regex formulaire et suppression des images inutiles
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drakmirr\Desktop\P5OC\JWDP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D4B885-D1EF-4FC4-8FE2-43C24A3C70B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E3975C-D5C5-41B0-B00C-0F8F367B5D05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3855" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -43,9 +43,6 @@
     <t>5 à 20</t>
   </si>
   <si>
-    <t>getAllCam</t>
-  </si>
-  <si>
     <t>cams</t>
   </si>
   <si>
@@ -121,15 +118,6 @@
     <t>La fonction envoi une requete API POST et doit retourner un objet contact avec l'orderId</t>
   </si>
   <si>
-    <t>retourner dans un console.log l'etat de la requete à l'aide la propriété readystate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reponse retourné differente 4 correspondant à une mauvaise connexion ou autre selon le status </t>
-  </si>
-  <si>
-    <t>liste2.js</t>
-  </si>
-  <si>
     <t>creationElementListe</t>
   </si>
   <si>
@@ -193,18 +181,12 @@
     <t>13 à 59</t>
   </si>
   <si>
-    <t>la fonction appel les 4 fonctions necessaires à la creation des cards</t>
-  </si>
-  <si>
     <t>verifier l'affichage des cards sur la page web</t>
   </si>
   <si>
     <t>mauvais affichage ou affichage absent des cards</t>
   </si>
   <si>
-    <t>panier3.js</t>
-  </si>
-  <si>
     <t>verifier l'existence l'objet dans le localstorage</t>
   </si>
   <si>
@@ -274,18 +256,12 @@
     <t>verifier le contenu de l'objeet produit</t>
   </si>
   <si>
-    <t>la fonction fait appel aux 5 fonctions necessaires à la creation du tableau</t>
-  </si>
-  <si>
     <t>verifier sur la page web l'affichage et le contenu du tableau</t>
   </si>
   <si>
     <t>mauvais affichage ou affichage absent du tableau</t>
   </si>
   <si>
-    <t>produitCard.js</t>
-  </si>
-  <si>
     <t>attributCardProduit</t>
   </si>
   <si>
@@ -307,27 +283,18 @@
     <t>12 à 41</t>
   </si>
   <si>
-    <t xml:space="preserve">la fonction appel 3 fonctions necessaires à l'affichage de la card </t>
-  </si>
-  <si>
     <t>verifier l'affichage de la card sur la page web</t>
   </si>
   <si>
     <t>affichage défaillant ou absent sur la page web</t>
   </si>
   <si>
-    <t>formulaire2.js</t>
-  </si>
-  <si>
     <t>verifInput</t>
   </si>
   <si>
     <t>21 à 30</t>
   </si>
   <si>
-    <t>La fonction doit vérifier le bon formatage des données de l'input ert affiche la couleur correspondante vert ou rouge</t>
-  </si>
-  <si>
     <t>on saisi des mots dans l'input pour verifier la couleur affichée</t>
   </si>
   <si>
@@ -379,7 +346,41 @@
     <t>a modifier précision</t>
   </si>
   <si>
-    <t>nommer les 4 fonctions</t>
+    <t>connectApi</t>
+  </si>
+  <si>
+    <t>la fonction fait appel aux 5 fonctions necessaires à la creation du tableau : creationElementPanier(); positionHtmlPanier(); ajoutAttributs(); ajoutContenuCellule(); ajoutContenuPanier();</t>
+  </si>
+  <si>
+    <t>La fonction appel les 4 fonctions necessaires à la creation des cards : creationElementListe();
+    ajoutAttributsCardListe()
+    positionHtml();
+    ajoutContenuCardListe();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La fonction appel 2 fonctions necessaires à l'affichage de la card :    attributCardProduit(infoCam);
+    ajoutContenuProduitCard(infoCam); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">une mauvaise connexion  </t>
+  </si>
+  <si>
+    <t>retourner la reponse dans un console.log</t>
+  </si>
+  <si>
+    <t>liste.js</t>
+  </si>
+  <si>
+    <t>panier.js</t>
+  </si>
+  <si>
+    <t>formulaire.js</t>
+  </si>
+  <si>
+    <t>produit.js</t>
+  </si>
+  <si>
+    <t>La fonction doit vérifier le bon formatage des données de l'input en affichant la couleur correspondante vert ou rouge</t>
   </si>
 </sst>
 </file>
@@ -501,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,6 +537,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,8 +759,8 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -818,485 +820,483 @@
     </row>
     <row r="3" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>119</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>96</v>
-      </c>
       <c r="F21" s="7" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
modification de envoiApi.js pour supprimer la dependance de l'objetdeRequete avec panier.js
</commit_message>
<xml_diff>
--- a/Plan de test.xlsx
+++ b/Plan de test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drakmirr\Desktop\P5OC\JWDP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E3975C-D5C5-41B0-B00C-0F8F367B5D05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512656A3-FBA5-4289-8D35-76F48681790B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3855" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="118">
   <si>
     <t>Fichier JS</t>
   </si>
@@ -341,9 +341,6 @@
   </si>
   <si>
     <t>l'orderId n'est pas recupérer et/ou n'est pas afficher</t>
-  </si>
-  <si>
-    <t>a modifier précision</t>
   </si>
   <si>
     <t>connectApi</t>
@@ -387,7 +384,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -418,8 +415,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,6 +478,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -499,10 +508,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,9 +547,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -760,7 +774,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -826,24 +840,22 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>113</v>
+      <c r="E3" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>107</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -863,7 +875,7 @@
     </row>
     <row r="5" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -883,7 +895,7 @@
     </row>
     <row r="6" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -903,7 +915,7 @@
     </row>
     <row r="7" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
@@ -923,7 +935,7 @@
     </row>
     <row r="8" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
         <v>52</v>
@@ -932,7 +944,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>53</v>
@@ -944,7 +956,7 @@
     </row>
     <row r="9" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -964,7 +976,7 @@
     </row>
     <row r="10" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -984,7 +996,7 @@
     </row>
     <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1004,7 +1016,7 @@
     </row>
     <row r="12" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1024,7 +1036,7 @@
     </row>
     <row r="13" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>67</v>
@@ -1044,7 +1056,7 @@
     </row>
     <row r="14" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>69</v>
@@ -1064,7 +1076,7 @@
     </row>
     <row r="15" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>70</v>
@@ -1084,7 +1096,7 @@
     </row>
     <row r="16" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>73</v>
@@ -1104,7 +1116,7 @@
     </row>
     <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>75</v>
@@ -1124,13 +1136,13 @@
     </row>
     <row r="18" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>78</v>
@@ -1141,7 +1153,7 @@
     </row>
     <row r="19" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>82</v>
@@ -1161,7 +1173,7 @@
     </row>
     <row r="20" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>83</v>
@@ -1181,7 +1193,7 @@
     </row>
     <row r="21" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>86</v>
@@ -1190,7 +1202,7 @@
         <v>16</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>87</v>
@@ -1201,7 +1213,7 @@
     </row>
     <row r="22" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>90</v>
@@ -1210,7 +1222,7 @@
         <v>89</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>91</v>
@@ -1221,7 +1233,7 @@
     </row>
     <row r="23" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>93</v>
@@ -1241,7 +1253,7 @@
     </row>
     <row r="24" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>98</v>

</xml_diff>